<commit_message>
Cell chrono + timer
</commit_message>
<xml_diff>
--- a/EL_Electrical/Cellule chrono/Scheme.xlsx
+++ b/EL_Electrical/Cellule chrono/Scheme.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arthu\Documents\Ressources2020\EL_Electrical\Cellule chrono\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A1E9B0-6014-49AF-AFFF-AB41A7E76F40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{798F2D1D-CC82-4F6D-9019-E654B899FB58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{F520CC6F-F712-4636-9B07-CFBBFE9FABF0}"/>
+    <workbookView xWindow="-11268" yWindow="576" windowWidth="23040" windowHeight="12204" xr2:uid="{F520CC6F-F712-4636-9B07-CFBBFE9FABF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
   <si>
     <t>TX1</t>
   </si>
@@ -237,7 +237,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,18 +259,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -299,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -323,21 +311,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -752,7 +733,7 @@
   <dimension ref="A1:AF20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AH9" sqref="AH9"/>
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -762,39 +743,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
+      <c r="A1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
       <c r="AB1" t="s">
         <v>33</v>
       </c>
-      <c r="AC1" s="11" t="s">
+      <c r="AC1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="AD1" s="11" t="s">
+      <c r="AD1" s="9" t="s">
         <v>32</v>
       </c>
       <c r="AF1" t="s">
@@ -802,15 +783,15 @@
       </c>
     </row>
     <row r="2" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
-      <c r="Z2" s="14"/>
+      <c r="A2" s="11"/>
+      <c r="Z2" s="11"/>
       <c r="AB2" t="s">
         <v>34</v>
       </c>
-      <c r="AC2" s="11" t="s">
+      <c r="AC2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="AD2" s="11" t="s">
+      <c r="AD2" s="9" t="s">
         <v>32</v>
       </c>
       <c r="AF2" t="s">
@@ -818,7 +799,7 @@
       </c>
     </row>
     <row r="3" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
+      <c r="A3" s="11"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
@@ -844,14 +825,14 @@
       <c r="Y3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="Z3" s="14"/>
+      <c r="Z3" s="11"/>
       <c r="AB3" t="s">
         <v>35</v>
       </c>
-      <c r="AC3" s="11" t="s">
+      <c r="AC3" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="AD3" s="11" t="s">
+      <c r="AD3" s="9" t="s">
         <v>32</v>
       </c>
       <c r="AF3" t="s">
@@ -859,7 +840,7 @@
       </c>
     </row>
     <row r="4" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
+      <c r="A4" s="11"/>
       <c r="I4" s="8"/>
       <c r="M4" s="2"/>
       <c r="N4" s="4" t="s">
@@ -882,125 +863,95 @@
       <c r="Y4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="Z4" s="14"/>
+      <c r="Z4" s="11"/>
       <c r="AF4" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
+      <c r="A5" s="11"/>
       <c r="I5" s="8"/>
       <c r="M5" s="2"/>
       <c r="Y5" s="1"/>
-      <c r="Z5" s="14"/>
+      <c r="Z5" s="11"/>
       <c r="AB5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
+      <c r="A6" s="11"/>
       <c r="I6" s="8"/>
       <c r="M6" s="2"/>
-      <c r="N6" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="O6" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="P6" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q6" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="R6" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="S6" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="T6" s="13" t="s">
+      <c r="V6" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="U6" s="13" t="s">
+      <c r="W6" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="X6" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y6" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="V6" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="W6" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="14"/>
+      <c r="Z6" s="11"/>
       <c r="AB6" t="s">
         <v>39</v>
       </c>
-      <c r="AC6" s="11" t="s">
+      <c r="AC6" s="9" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
+      <c r="A7" s="11"/>
       <c r="I7" s="8"/>
       <c r="M7" s="2"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
+      <c r="P7" s="12"/>
       <c r="Q7" s="12"/>
       <c r="R7" s="12"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="15"/>
-      <c r="U7" s="15"/>
-      <c r="V7" s="15"/>
-      <c r="Z7" s="14"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="W7" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="X7" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y7" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z7" s="11"/>
       <c r="AB7" t="s">
         <v>40</v>
       </c>
-      <c r="AC7" s="11" t="s">
+      <c r="AC7" s="9" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
+      <c r="A8" s="11"/>
       <c r="I8" s="8"/>
       <c r="M8" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="N8" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="O8" s="10" t="s">
-        <v>29</v>
-      </c>
       <c r="P8" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="Q8" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R8" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="S8" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="T8" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="U8" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="V8" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="W8" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z8" s="14"/>
+      <c r="W8" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="X8" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y8" s="12"/>
+      <c r="Z8" s="11"/>
     </row>
     <row r="9" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
+      <c r="A9" s="11"/>
       <c r="I9" s="8"/>
       <c r="J9" s="6" t="s">
         <v>0</v>
@@ -1047,8 +998,8 @@
       <c r="X9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="14"/>
+      <c r="Y9" s="12"/>
+      <c r="Z9" s="11"/>
       <c r="AB9" t="s">
         <v>46</v>
       </c>
@@ -1057,13 +1008,11 @@
       </c>
     </row>
     <row r="10" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14"/>
+      <c r="A10" s="11"/>
       <c r="I10" s="8"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -1075,8 +1024,8 @@
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="14"/>
+      <c r="Y10" s="12"/>
+      <c r="Z10" s="11"/>
       <c r="AB10" t="s">
         <v>41</v>
       </c>
@@ -1085,14 +1034,14 @@
       </c>
     </row>
     <row r="11" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14"/>
+      <c r="A11" s="11"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
-      <c r="M11" s="2"/>
+      <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
@@ -1102,15 +1051,15 @@
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
-      <c r="W11" s="16" t="s">
+      <c r="W11" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="X11" s="16"/>
-      <c r="Y11" s="16"/>
-      <c r="Z11" s="16"/>
+      <c r="X11" s="13"/>
+      <c r="Y11" s="13"/>
+      <c r="Z11" s="13"/>
     </row>
     <row r="12" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14"/>
+      <c r="A12" s="11"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1118,7 +1067,7 @@
       <c r="J12" s="5"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="2"/>
+      <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -1128,10 +1077,10 @@
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
-      <c r="W12" s="16"/>
-      <c r="X12" s="16"/>
-      <c r="Y12" s="16"/>
-      <c r="Z12" s="16"/>
+      <c r="W12" s="13"/>
+      <c r="X12" s="13"/>
+      <c r="Y12" s="13"/>
+      <c r="Z12" s="13"/>
       <c r="AB12" t="s">
         <v>42</v>
       </c>
@@ -1140,7 +1089,7 @@
       </c>
     </row>
     <row r="13" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
+      <c r="A13" s="11"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1150,7 +1099,7 @@
       <c r="J13" s="5"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="2"/>
+      <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -1160,13 +1109,13 @@
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
-      <c r="W13" s="16"/>
-      <c r="X13" s="16"/>
-      <c r="Y13" s="16"/>
-      <c r="Z13" s="16"/>
+      <c r="W13" s="13"/>
+      <c r="X13" s="13"/>
+      <c r="Y13" s="13"/>
+      <c r="Z13" s="13"/>
     </row>
     <row r="14" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="14"/>
+      <c r="A14" s="11"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="4" t="s">
@@ -1180,8 +1129,8 @@
       <c r="K14" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -1192,12 +1141,14 @@
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
-      <c r="X14" s="1"/>
-      <c r="Y14" s="1"/>
-      <c r="Z14" s="14"/>
+      <c r="X14" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y14" s="12"/>
+      <c r="Z14" s="11"/>
     </row>
     <row r="15" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="14"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1258,10 +1209,10 @@
         <v>27</v>
       </c>
       <c r="Y15" s="1"/>
-      <c r="Z15" s="14"/>
+      <c r="Z15" s="11"/>
     </row>
     <row r="16" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="14"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1270,10 +1221,10 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-      <c r="Z16" s="14"/>
+      <c r="Z16" s="11"/>
     </row>
     <row r="17" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="14"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1281,10 +1232,10 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="Z17" s="14"/>
+      <c r="Z17" s="11"/>
     </row>
     <row r="18" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="14"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1292,45 +1243,45 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="Z18" s="14"/>
+      <c r="Z18" s="11"/>
     </row>
     <row r="19" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="14"/>
+      <c r="A19" s="11"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="Z19" s="14"/>
+      <c r="Z19" s="11"/>
     </row>
     <row r="20" spans="1:26" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="14"/>
-      <c r="R20" s="14"/>
-      <c r="S20" s="14"/>
-      <c r="T20" s="14"/>
-      <c r="U20" s="14"/>
-      <c r="V20" s="14"/>
-      <c r="W20" s="14"/>
-      <c r="X20" s="14"/>
-      <c r="Y20" s="14"/>
-      <c r="Z20" s="14"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="11"/>
+      <c r="V20" s="11"/>
+      <c r="W20" s="11"/>
+      <c r="X20" s="11"/>
+      <c r="Y20" s="11"/>
+      <c r="Z20" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>